<commit_message>
revised family profile UI
</commit_message>
<xml_diff>
--- a/capstone/files/fhsis/28.xlsx
+++ b/capstone/files/fhsis/28.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmlon\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmlon\Documents\Capstone\Likha-Capstone\capstone\files\fhsis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{032468C7-5481-4128-8EB0-459965DAC308}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B2ED6F1-185F-4C57-A064-B75D35A8F2CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{3D0A857D-EDBF-46E0-B380-6A5DDAD258B4}"/>
   </bookViews>
@@ -328,10 +328,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -339,6 +335,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
   </cellXfs>
@@ -657,8 +657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A393474-95DC-4EE8-BFB9-DD78CCDF7A0E}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,21 +668,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="15"/>
     </row>
     <row r="4" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="22" t="s">
+      <c r="A4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -707,7 +707,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -765,25 +765,25 @@
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="21"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="21"/>
-      <c r="O16" s="21"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
     </row>
     <row r="17" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="25" t="s">
+      <c r="A17" s="23"/>
+      <c r="B17" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="9"/>

</xml_diff>